<commit_message>
last updates 14:40 25.09.2021
</commit_message>
<xml_diff>
--- a/plugins/exelphp/result/kvitansiya.xlsx
+++ b/plugins/exelphp/result/kvitansiya.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>СУММА</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Тулов тури:</t>
   </si>
   <si>
-    <t>Plastik</t>
+    <t>Naqd</t>
   </si>
   <si>
     <t>Бошқа тушумлар №1-100 шартнома асаосан ўтказилди</t>
@@ -89,13 +89,16 @@
     <t>________________</t>
   </si>
   <si>
-    <t>Naqd</t>
-  </si>
-  <si>
     <t>КВИТАНЦИЯ №</t>
   </si>
   <si>
     <t>001-шакл</t>
+  </si>
+  <si>
+    <t>Рахмонова  Гулсора Абдулхакимовна</t>
+  </si>
+  <si>
+    <t>245 000,00</t>
   </si>
   <si>
     <t>х/в</t>
@@ -1352,7 +1355,7 @@
   <dimension ref="A1:AF61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="115" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1400,7 +1403,9 @@
       <c r="F1" s="175"/>
       <c r="G1" s="69"/>
       <c r="H1" s="69"/>
-      <c r="I1" s="183"/>
+      <c r="I1" s="183">
+        <v>100</v>
+      </c>
       <c r="J1" s="184"/>
       <c r="K1" s="57"/>
       <c r="L1" s="7"/>
@@ -1546,7 +1551,7 @@
       <c r="F5" s="106"/>
       <c r="G5" s="105"/>
       <c r="H5" s="156">
-        <v>500000</v>
+        <v>1095000</v>
       </c>
       <c r="I5" s="156"/>
       <c r="J5" s="157"/>
@@ -1910,9 +1915,7 @@
       <c r="G14" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="72" t="s">
-        <v>23</v>
-      </c>
+      <c r="H14" s="72"/>
       <c r="I14" s="27"/>
       <c r="J14" s="28"/>
       <c r="K14" s="25" t="s">
@@ -2014,7 +2017,7 @@
       <c r="I17" s="59"/>
       <c r="J17" s="31"/>
       <c r="K17" s="51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L17" s="50"/>
       <c r="M17" s="50"/>
@@ -2024,7 +2027,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="131" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T17" s="132"/>
       <c r="V17" s="48"/>
@@ -2109,17 +2112,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="142"/>
-      <c r="C20" s="105" t="str">
-        <f>C5</f>
-        <v>0</v>
+      <c r="C20" s="105" t="s">
+        <v>25</v>
       </c>
       <c r="D20" s="105"/>
       <c r="E20" s="106"/>
       <c r="F20" s="106"/>
       <c r="G20" s="105"/>
-      <c r="H20" s="156" t="str">
-        <f>H5</f>
-        <v>0</v>
+      <c r="H20" s="156" t="s">
+        <v>26</v>
       </c>
       <c r="I20" s="156"/>
       <c r="J20" s="157"/>
@@ -2231,7 +2232,7 @@
       </c>
       <c r="B23" s="143"/>
       <c r="C23" s="128" t="str">
-        <f>C8</f>
+        <f>C20</f>
         <v>0</v>
       </c>
       <c r="D23" s="129"/>
@@ -2242,7 +2243,7 @@
       <c r="I23" s="159"/>
       <c r="J23" s="160"/>
       <c r="K23" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L23" s="16" t="str">
         <f>L6</f>
@@ -2273,9 +2274,8 @@
         <v>12</v>
       </c>
       <c r="B24" s="167"/>
-      <c r="C24" s="102" t="str">
-        <f>C9</f>
-        <v>0</v>
+      <c r="C24" s="102">
+        <v>75555</v>
       </c>
       <c r="D24" s="102"/>
       <c r="E24" s="102"/>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="L24" s="147"/>
       <c r="M24" s="100" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N24" s="100"/>
       <c r="O24" s="101"/>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="B25" s="145"/>
       <c r="C25" s="162" t="str">
-        <f>C10</f>
+        <f>UPPER(LEFT(Formula!B20,1))&amp;RIGHT(Formula!B20,LEN(Formula!B20)-1)</f>
         <v>0</v>
       </c>
       <c r="D25" s="163"/>
@@ -3122,60 +3122,60 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="C1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:25">

</xml_diff>